<commit_message>
fix(pipelining): fix reading Rm from the register file #2
</commit_message>
<xml_diff>
--- a/programs/fpumaclaurinprogramsinpiover2.xlsx
+++ b/programs/fpumaclaurinprogramsinpiover2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4C1615-983B-4A60-8AA0-C82B09F7C9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925B491B-714C-4DEE-B184-A8F43832CE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
@@ -883,8 +883,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+    <sheetView tabSelected="1" topLeftCell="M10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>